<commit_message>
Añdiendo resultados del anaisis de datos
</commit_message>
<xml_diff>
--- a/datos/datos_benchmark.xlsx
+++ b/datos/datos_benchmark.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
   <si>
     <t xml:space="preserve">Pc/computadora</t>
   </si>
@@ -83,6 +83,21 @@
   </si>
   <si>
     <t xml:space="preserve">Media Aritmética</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datos normalizados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referencia: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiempo de respuesta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media geométrica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desempeño</t>
   </si>
 </sst>
 </file>
@@ -200,12 +215,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -278,12 +293,13 @@
   <dimension ref="A2:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -568,6 +584,359 @@
       <c r="G12" s="4" t="n">
         <f aca="false">AVERAGE(B12:F12)</f>
         <v>1758795.322</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <f aca="false">B3/B3</f>
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <f aca="false">C3/C3</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <f aca="false">D3/D3</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <f aca="false">E3/E3</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">F3/F3</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <f aca="false">G3/G3</f>
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <f aca="false">H3/H3</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <f aca="false">I3/I3</f>
+        <v>1</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <f aca="false">GEOMEAN(B17:I17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <f aca="false">B4/B3</f>
+        <v>0.0138283765864747</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <f aca="false">C4/C3</f>
+        <v>0.658722524169112</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="false">D4/D3</f>
+        <v>0.80841169784024</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <f aca="false">E4/E3</f>
+        <v>0.799811001691037</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <f aca="false">F4/F3</f>
+        <v>1.13238289205703</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <f aca="false">G4/G3</f>
+        <v>1.11853043711451</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <f aca="false">H4/H3</f>
+        <v>0.890014471780029</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <f aca="false">I4/I3</f>
+        <v>0.74021658100208</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <f aca="false">GEOMEAN(B18:I18)</f>
+        <v>0.514560366776574</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <f aca="false">B5/B3</f>
+        <v>0.00826387573404054</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <f aca="false">C5/C3</f>
+        <v>0.354720792650666</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="false">D5/D3</f>
+        <v>0.614756639454376</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <f aca="false">E5/E3</f>
+        <v>0.337511190689346</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">F5/F3</f>
+        <v>0.451007015161801</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <f aca="false">G5/G3</f>
+        <v>0.509251810136766</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <f aca="false">H5/H3</f>
+        <v>0.405571635311143</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <f aca="false">I5/I3</f>
+        <v>0.299364381841723</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <f aca="false">GEOMEAN(B19:I19)</f>
+        <v>0.253326531029157</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <f aca="false">B6/B3</f>
+        <v>0.00672475847698428</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <f aca="false">C6/C3</f>
+        <v>0.261976335914578</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <f aca="false">D6/D3</f>
+        <v>0.491164617133409</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <f aca="false">E6/E3</f>
+        <v>0.266388142842932</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <f aca="false">F6/F3</f>
+        <v>0.305272686128083</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <f aca="false">G6/G3</f>
+        <v>0.382408152319657</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <f aca="false">H6/H3</f>
+        <v>0.315846599131693</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <f aca="false">I6/I3</f>
+        <v>0.245281908423902</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <f aca="false">GEOMEAN(B20:I20)</f>
+        <v>0.194930452635808</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <f aca="false">B9/B9</f>
+        <v>1</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <f aca="false">C9/C9</f>
+        <v>1</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <f aca="false">D9/D9</f>
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <f aca="false">E9/E9</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <f aca="false">F9/F9</f>
+        <v>1</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <f aca="false">GEOMEAN(B24:F24)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <f aca="false">B10/B9</f>
+        <v>1.78717056350907</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <f aca="false">C10/C9</f>
+        <v>1.71032619851656</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <f aca="false">D10/D9</f>
+        <v>1.59053304800192</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <f aca="false">E10/E9</f>
+        <v>1.87154366813972</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <f aca="false">F10/F9</f>
+        <v>1.77898080607844</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <f aca="false">GEOMEAN(B25:F25)</f>
+        <v>1.74514603574744</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <f aca="false">B11/B9</f>
+        <v>2.18938659519946</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <f aca="false">C11/C9</f>
+        <v>2.39240389874254</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <f aca="false">D11/D9</f>
+        <v>2.82792898754977</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <f aca="false">E11/E9</f>
+        <v>2.71988900165419</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <f aca="false">F11/F9</f>
+        <v>2.62690020375596</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">GEOMEAN(B26:F26)</f>
+        <v>2.54052833000873</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <f aca="false">B12/B9</f>
+        <v>3.82234470158343</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <f aca="false">C12/C9</f>
+        <v>3.98026987714027</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <f aca="false">D12/D9</f>
+        <v>4.36096413007475</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <f aca="false">E12/E9</f>
+        <v>4.26225456899238</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <f aca="false">F12/F9</f>
+        <v>4.11993440052126</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <f aca="false">GEOMEAN(B27:F27)</f>
+        <v>4.10460069149026</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Datos ponderados a las tablas de Excel
</commit_message>
<xml_diff>
--- a/datos/datos_benchmark.xlsx
+++ b/datos/datos_benchmark.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="32">
   <si>
     <t xml:space="preserve">Pc/computadora</t>
   </si>
@@ -98,6 +98,24 @@
   </si>
   <si>
     <t xml:space="preserve">Desempeño</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medidas ponderadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pesos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computadora (inv)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computadora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media armónica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media aritmética</t>
   </si>
 </sst>
 </file>
@@ -293,12 +311,12 @@
   <dimension ref="A2:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
@@ -937,6 +955,361 @@
       <c r="G27" s="0" t="n">
         <f aca="false">GEOMEAN(B27:F27)</f>
         <v>4.10460069149026</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <f aca="false">1/B3</f>
+        <v>0.00236787270316348</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <f aca="false">1/C3</f>
+        <v>0.00120244336491751</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <f aca="false">1/D3</f>
+        <v>0.0103337811305157</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <f aca="false">1/E3</f>
+        <v>0.00497363970953944</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <f aca="false">1/F3</f>
+        <v>0.0226295541977823</v>
+      </c>
+      <c r="G35" s="0" t="n">
+        <f aca="false">1/G3</f>
+        <v>0.026816840976133</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <f aca="false">1/H3</f>
+        <v>0.0361794500723589</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <f aca="false">1/I3</f>
+        <v>0.000392356887825166</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <f aca="false">1/B4</f>
+        <v>0.171232876712329</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <f aca="false">1/C4</f>
+        <v>0.00182541710780913</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <f aca="false">1/D4</f>
+        <v>0.0127828198900677</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <f aca="false">1/E4</f>
+        <v>0.00621851874883403</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <f aca="false">1/F4</f>
+        <v>0.0199840127897682</v>
+      </c>
+      <c r="G36" s="0" t="n">
+        <f aca="false">1/G4</f>
+        <v>0.0239750659314313</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <f aca="false">1/H4</f>
+        <v>0.040650406504065</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <f aca="false">1/I4</f>
+        <v>0.000530056875102699</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <f aca="false">1/B5</f>
+        <v>0.286532951289398</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <f aca="false">1/C5</f>
+        <v>0.00338983050847458</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <f aca="false">1/D5</f>
+        <v>0.0168095478231636</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <f aca="false">1/E5</f>
+        <v>0.0147362216327734</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <f aca="false">1/F5</f>
+        <v>0.0501756146512795</v>
+      </c>
+      <c r="G37" s="0" t="n">
+        <f aca="false">1/G5</f>
+        <v>0.0526592943654555</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <f aca="false">1/H5</f>
+        <v>0.0892060660124889</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <f aca="false">1/I5</f>
+        <v>0.00131063316688292</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <f aca="false">1/B6</f>
+        <v>0.352112676056338</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <f aca="false">1/C6</f>
+        <v>0.00458989305549181</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <f aca="false">1/D6</f>
+        <v>0.0210393435724805</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <f aca="false">1/E6</f>
+        <v>0.0186706497386109</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <f aca="false">1/F6</f>
+        <v>0.0741289844329133</v>
+      </c>
+      <c r="G38" s="0" t="n">
+        <f aca="false">1/G6</f>
+        <v>0.0701262272089762</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <f aca="false">1/H6</f>
+        <v>0.11454753722795</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <f aca="false">1/I6</f>
+        <v>0.00159961609213789</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <f aca="false">SUM(B32:I32)/SUMPRODUCT(B32:I32, B35:I35)</f>
+        <v>129.379742225352</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <f aca="false">SUM(B32:I32)/SUMPRODUCT(B32:I32, B36:I36)</f>
+        <v>23.1993219253364</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <f aca="false">SUM(B32:I32)/SUMPRODUCT(B32:I32, B37:I37)</f>
+        <v>13.2294491005755</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <f aca="false">SUM(B32:I32)/SUMPRODUCT(B32:I32, B38:I38)</f>
+        <v>10.5541413519385</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="E51" s="0" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="F51" s="0" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <f aca="false">SUMPRODUCT(B9:F9, B51:F51)</f>
+        <v>432723.55</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <f aca="false">SUMPRODUCT(B10:F10, B51:F51)</f>
+        <v>764760.016</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <f aca="false">SUMPRODUCT(B11:F11, B51:F51)</f>
+        <v>1077350.66</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <f aca="false">SUMPRODUCT(B12:F12, B51:F51)</f>
+        <v>1754442.2645</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Corrigiendo peso en tiempos de respuesta
</commit_message>
<xml_diff>
--- a/datos/datos_benchmark.xlsx
+++ b/datos/datos_benchmark.xlsx
@@ -310,8 +310,8 @@
   </sheetPr>
   <dimension ref="A2:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44:B47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1019,7 +1019,7 @@
         <v>0.05</v>
       </c>
       <c r="I32" s="0" t="n">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="B44" s="0" t="n">
         <f aca="false">SUM(B32:I32)/SUMPRODUCT(B32:I32, B35:I35)</f>
-        <v>129.379742225352</v>
+        <v>108.736416907889</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,7 +1203,7 @@
       </c>
       <c r="B45" s="0" t="n">
         <f aca="false">SUM(B32:I32)/SUMPRODUCT(B32:I32, B36:I36)</f>
-        <v>23.1993219253364</v>
+        <v>19.3724720236483</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="B46" s="0" t="n">
         <f aca="false">SUM(B32:I32)/SUMPRODUCT(B32:I32, B37:I37)</f>
-        <v>13.2294491005755</v>
+        <v>11.0564922536646</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B47" s="0" t="n">
         <f aca="false">SUM(B32:I32)/SUMPRODUCT(B32:I32, B38:I38)</f>
-        <v>10.5541413519385</v>
+        <v>8.81993499466002</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>